<commit_message>
new changes in Feature + Bulk File
</commit_message>
<xml_diff>
--- a/src/test/TestData/MasterDataSheet.xlsx
+++ b/src/test/TestData/MasterDataSheet.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development_venus\WorkSpace_1\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93351A01-779A-44BF-8A97-FB1AC80827C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2812FD-9740-45F8-A0A6-11BB8B3AFE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC_001" sheetId="2" r:id="rId1"/>
     <sheet name="TC_002" sheetId="3" r:id="rId2"/>
     <sheet name="TC_010" sheetId="9" r:id="rId3"/>
+    <sheet name="Owner" sheetId="10" r:id="rId4"/>
+    <sheet name="Admin" sheetId="11" r:id="rId5"/>
+    <sheet name="Student" sheetId="12" r:id="rId6"/>
+    <sheet name="Lecturer" sheetId="13" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="618">
   <si>
     <t>Variable</t>
   </si>
@@ -1539,9 +1543,6 @@
   </si>
   <si>
     <t>drp_Students</t>
-  </si>
-  <si>
-    <t>priya lecturer</t>
   </si>
   <si>
     <t>drp_Assigncourse</t>
@@ -1704,12 +1705,6 @@
   </si>
   <si>
     <t>btn_CourseDelete</t>
-  </si>
-  <si>
-    <t>mKfKW:mKfKW:</t>
-  </si>
-  <si>
-    <t>clientuser03lgim@gmail.com</t>
   </si>
   <si>
     <t>txt_UpdateAssignment Title</t>
@@ -1769,12 +1764,144 @@
   <si>
     <t>Assignment 0002</t>
   </si>
+  <si>
+    <t>priya student 01</t>
+  </si>
+  <si>
+    <t>clientuser02lgim@gmail.com</t>
+  </si>
+  <si>
+    <t>8QWoi98QWoi9</t>
+  </si>
+  <si>
+    <t>//a[@href='/app/management/users']</t>
+  </si>
+  <si>
+    <t>btn_Users</t>
+  </si>
+  <si>
+    <t>btn_Administrator</t>
+  </si>
+  <si>
+    <t>btn_Administratorlist</t>
+  </si>
+  <si>
+    <t>//button[text()='Administrators']</t>
+  </si>
+  <si>
+    <t>//span[text()='Administrator']</t>
+  </si>
+  <si>
+    <t>//span[text()='Student']</t>
+  </si>
+  <si>
+    <t>//span[text()='Lecturer']</t>
+  </si>
+  <si>
+    <t>//button[text()='Students']</t>
+  </si>
+  <si>
+    <t>btn_Lecturer</t>
+  </si>
+  <si>
+    <t>btn_Lecturerlist</t>
+  </si>
+  <si>
+    <t>btn_Student</t>
+  </si>
+  <si>
+    <t>btn_Studentlist</t>
+  </si>
+  <si>
+    <t>//button[text()='Lecturers']</t>
+  </si>
+  <si>
+    <t>priyaganasalesforce@gmail.com</t>
+  </si>
+  <si>
+    <t>965600v</t>
+  </si>
+  <si>
+    <t>Yi:bzYYi:bzY</t>
+  </si>
+  <si>
+    <t>clientuser03lgim@gmail.com</t>
+  </si>
+  <si>
+    <t>btn_tableCourse</t>
+  </si>
+  <si>
+    <t>//th[text()='Course']</t>
+  </si>
+  <si>
+    <t>//li[text()='Delete']</t>
+  </si>
+  <si>
+    <t>file_SubmitAssignmentMeterial</t>
+  </si>
+  <si>
+    <t>//*[@class="MuiButtonBase-root MuiButton-root MuiButton-contained MuiButton-containedSecondary MuiButton-sizeMedium MuiButton-containedSizeMedium MuiButton-fullWidth  css-1bpzmgq"]</t>
+  </si>
+  <si>
+    <t>//*[text()='Submit']</t>
+  </si>
+  <si>
+    <t>btn_AssignmentSubmit</t>
+  </si>
+  <si>
+    <t>btn_EditAssignmentSubmit</t>
+  </si>
+  <si>
+    <t>//*[text()='Edit Submission']</t>
+  </si>
+  <si>
+    <t>file_EditSubmitAssignmentMeterial</t>
+  </si>
+  <si>
+    <t>//*[text()='Grade']</t>
+  </si>
+  <si>
+    <t>btn_Grade</t>
+  </si>
+  <si>
+    <t>txt_Feedback</t>
+  </si>
+  <si>
+    <t>txt_Marks</t>
+  </si>
+  <si>
+    <t>//*[@name="feedback"]</t>
+  </si>
+  <si>
+    <t>//*[@name="marks"]</t>
+  </si>
+  <si>
+    <t>``</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>btn_EditGrade</t>
+  </si>
+  <si>
+    <t>txt_EditFeedback</t>
+  </si>
+  <si>
+    <t>txt_EditMarks</t>
+  </si>
+  <si>
+    <t>Poor</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1864,8 +1991,44 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1920,6 +2083,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1949,7 +2148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2011,6 +2210,60 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="18" fillId="12" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="18" fillId="15" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2396,18 +2649,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="43.85546875" customWidth="1"/>
     <col min="2" max="2" width="101.7109375" customWidth="1"/>
     <col min="3" max="3" width="67.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2418,7 +2671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="16" t="s">
         <v>484</v>
       </c>
@@ -2429,7 +2682,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="16" t="s">
         <v>485</v>
       </c>
@@ -2440,7 +2693,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
@@ -2449,7 +2702,7 @@
       </c>
       <c r="C4" s="16"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="9" t="s">
         <v>486</v>
       </c>
@@ -2458,7 +2711,7 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="12" t="s">
         <v>489</v>
       </c>
@@ -2467,7 +2720,7 @@
       </c>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="12" t="s">
         <v>491</v>
       </c>
@@ -2478,7 +2731,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.75">
       <c r="A8" s="12" t="s">
         <v>493</v>
       </c>
@@ -2489,7 +2742,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.75">
       <c r="A9" s="12" t="s">
         <v>494</v>
       </c>
@@ -2497,10 +2750,10 @@
         <v>498</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="14" t="s">
         <v>497</v>
       </c>
@@ -2509,7 +2762,7 @@
       </c>
       <c r="C10" s="15"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15.75">
       <c r="A11" s="10" t="s">
         <v>500</v>
       </c>
@@ -2518,9 +2771,9 @@
       </c>
       <c r="C11" s="11"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15.75">
       <c r="A12" s="10" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>501</v>
@@ -2529,7 +2782,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15.75">
       <c r="A13" s="10" t="s">
         <v>503</v>
       </c>
@@ -2537,262 +2790,262 @@
         <v>502</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75">
       <c r="A14" s="17" t="s">
+        <v>506</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>517</v>
+      </c>
+      <c r="C14" s="18"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75">
+      <c r="A15" s="17" t="s">
         <v>507</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B15" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C15" s="18"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75">
+      <c r="A16" s="17" t="s">
+        <v>508</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>518</v>
       </c>
-      <c r="C14" s="18"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>508</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>506</v>
-      </c>
-      <c r="C15" s="18"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="C16" s="17" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75">
+      <c r="A17" s="17" t="s">
+        <v>510</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>509</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>519</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>511</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>510</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="17.25">
       <c r="A18" s="17" t="s">
+        <v>513</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>514</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>513</v>
-      </c>
-      <c r="C18" s="21" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="15.75">
+      <c r="A19" s="17" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="B19" s="19" t="s">
         <v>516</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>517</v>
-      </c>
       <c r="C19" s="19"/>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15.75">
       <c r="A20" s="17" t="s">
+        <v>530</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="C20" s="19"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="31" t="s">
+        <v>520</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>531</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>520</v>
-      </c>
-      <c r="C20" s="19"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="C21" s="22"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="31" t="s">
+        <v>524</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>505</v>
+      </c>
+      <c r="C22" s="22"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="31" t="s">
         <v>521</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>532</v>
-      </c>
-      <c r="C21" s="22"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
-        <v>525</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>506</v>
-      </c>
-      <c r="C22" s="22"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
-        <v>522</v>
       </c>
       <c r="B23" s="22" t="s">
         <v>492</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C24" s="22"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="31" t="s">
+        <v>525</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="C25" s="27" t="s">
         <v>526</v>
       </c>
-      <c r="B25" s="22" t="s">
-        <v>523</v>
-      </c>
-      <c r="C25" s="27" t="s">
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="31" t="s">
+        <v>528</v>
+      </c>
+      <c r="B26" s="31" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="C26" s="28" t="s">
         <v>529</v>
       </c>
-      <c r="B26" s="31" t="s">
-        <v>528</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" ht="60">
       <c r="A27" s="31" t="s">
+        <v>549</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="C27" s="29" t="s">
         <v>550</v>
       </c>
-      <c r="B27" s="22" t="s">
-        <v>549</v>
-      </c>
-      <c r="C27" s="29" t="s">
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="31" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
-        <v>552</v>
-      </c>
       <c r="B28" s="22" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C28" s="31" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="31" t="s">
+        <v>553</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>552</v>
+      </c>
+      <c r="C29" s="31"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="32" t="s">
+        <v>533</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>532</v>
+      </c>
+      <c r="C30" s="30"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75">
+      <c r="A31" s="23" t="s">
+        <v>537</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>534</v>
+      </c>
+      <c r="C31" s="24"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75">
+      <c r="A32" s="23" t="s">
+        <v>538</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>535</v>
+      </c>
+      <c r="C32" s="24"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75">
+      <c r="A33" s="23" t="s">
+        <v>539</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>536</v>
+      </c>
+      <c r="C33" s="24"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75">
+      <c r="A34" s="23" t="s">
         <v>554</v>
       </c>
-      <c r="B29" s="22" t="s">
-        <v>553</v>
-      </c>
-      <c r="C29" s="31"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
-        <v>534</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>533</v>
-      </c>
-      <c r="C30" s="30"/>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
-        <v>538</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>535</v>
-      </c>
-      <c r="C31" s="24"/>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
-        <v>539</v>
-      </c>
-      <c r="B32" s="24" t="s">
-        <v>536</v>
-      </c>
-      <c r="C32" s="24"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="23" t="s">
+      <c r="B34" s="24" t="s">
+        <v>518</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75">
+      <c r="A35" s="23" t="s">
         <v>540</v>
       </c>
-      <c r="B33" s="24" t="s">
-        <v>537</v>
-      </c>
-      <c r="C33" s="24"/>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
-        <v>555</v>
-      </c>
-      <c r="B34" s="24" t="s">
-        <v>519</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
-        <v>541</v>
-      </c>
       <c r="B35" s="24" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C35" s="25" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="17.25">
       <c r="A36" s="23" t="s">
+        <v>541</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>512</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75">
+      <c r="A37" s="23" t="s">
         <v>542</v>
       </c>
-      <c r="B36" s="24" t="s">
-        <v>513</v>
-      </c>
-      <c r="C36" s="26" t="s">
+      <c r="B37" s="24" t="s">
+        <v>571</v>
+      </c>
+      <c r="C37" s="24"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.75">
+      <c r="A38" s="23" t="s">
+        <v>546</v>
+      </c>
+      <c r="B38" s="24" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
-        <v>543</v>
-      </c>
-      <c r="B37" s="24" t="s">
-        <v>574</v>
-      </c>
-      <c r="C37" s="24"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
-        <v>547</v>
-      </c>
-      <c r="B38" s="24" t="s">
-        <v>546</v>
-      </c>
       <c r="C38" s="24"/>
     </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15.75">
       <c r="A39" s="33" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C39" s="34"/>
     </row>
@@ -2811,17 +3064,17 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A14" sqref="A14:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="80.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="45.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16.5" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2832,7 +3085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15">
       <c r="A2" s="16" t="s">
         <v>484</v>
       </c>
@@ -2840,10 +3093,10 @@
         <v>77</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" s="16" t="s">
         <v>485</v>
       </c>
@@ -2851,10 +3104,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
@@ -2863,7 +3116,7 @@
       </c>
       <c r="C4" s="16"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="9" t="s">
         <v>486</v>
       </c>
@@ -2872,332 +3125,332 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="17" t="s">
+        <v>506</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>517</v>
+      </c>
+      <c r="C6" s="18"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="17" t="s">
         <v>507</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B7" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C7" s="18"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="17" t="s">
+        <v>508</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>518</v>
       </c>
-      <c r="C6" s="18"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>508</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>506</v>
-      </c>
-      <c r="C7" s="18"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="C8" s="17" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="17" t="s">
+        <v>510</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>509</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>519</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>511</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>510</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="17.25">
       <c r="A10" s="17" t="s">
+        <v>513</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>514</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>513</v>
-      </c>
-      <c r="C10" s="21" t="s">
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="17" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="B11" s="19" t="s">
         <v>516</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>517</v>
-      </c>
       <c r="C11" s="19"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="17" t="s">
+        <v>530</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="C12" s="19"/>
+    </row>
+    <row r="13" spans="1:3" ht="15">
+      <c r="A13" s="31" t="s">
+        <v>520</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>531</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>520</v>
-      </c>
-      <c r="C12" s="19"/>
-    </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="C13" s="22"/>
+    </row>
+    <row r="14" spans="1:3" ht="15">
+      <c r="A14" s="31" t="s">
+        <v>524</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>505</v>
+      </c>
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" spans="1:3" ht="15">
+      <c r="A15" s="31" t="s">
         <v>521</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>532</v>
-      </c>
-      <c r="C13" s="22"/>
-    </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>525</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>506</v>
-      </c>
-      <c r="C14" s="22"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>522</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>492</v>
       </c>
       <c r="C15" s="22" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15">
+      <c r="A16" s="31" t="s">
+        <v>523</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="C16" s="22"/>
+    </row>
+    <row r="17" spans="1:3" ht="15">
+      <c r="A17" s="31" t="s">
+        <v>525</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15">
+      <c r="A18" s="31" t="s">
+        <v>528</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>527</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="60">
+      <c r="A19" s="31" t="s">
+        <v>549</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
-        <v>524</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>523</v>
-      </c>
-      <c r="C16" s="22"/>
-    </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
-        <v>526</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>523</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>529</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>528</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="C19" s="29" t="s">
         <v>550</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>549</v>
-      </c>
-      <c r="C19" s="29" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="15">
+      <c r="A20" s="31" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
-        <v>552</v>
-      </c>
       <c r="B20" s="22" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C20" s="31" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15">
       <c r="A21" s="31" t="s">
+        <v>553</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>552</v>
+      </c>
+      <c r="C21" s="31"/>
+    </row>
+    <row r="22" spans="1:3" ht="15">
+      <c r="A22" s="32" t="s">
+        <v>533</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>532</v>
+      </c>
+      <c r="C22" s="30"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="23" t="s">
+        <v>537</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>534</v>
+      </c>
+      <c r="C23" s="24"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="23" t="s">
+        <v>538</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>535</v>
+      </c>
+      <c r="C24" s="24"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="23" t="s">
+        <v>539</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>536</v>
+      </c>
+      <c r="C25" s="24"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="23" t="s">
         <v>554</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>553</v>
-      </c>
-      <c r="C21" s="31"/>
-    </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
-        <v>534</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>533</v>
-      </c>
-      <c r="C22" s="30"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
-        <v>538</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>535</v>
-      </c>
-      <c r="C23" s="24"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
-        <v>539</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>536</v>
-      </c>
-      <c r="C24" s="24"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="B26" s="24" t="s">
+        <v>518</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="23" t="s">
         <v>540</v>
       </c>
-      <c r="B25" s="24" t="s">
-        <v>537</v>
-      </c>
-      <c r="C25" s="24"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
-        <v>555</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>519</v>
-      </c>
-      <c r="C26" s="23" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
-        <v>541</v>
-      </c>
       <c r="B27" s="24" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="17.25">
       <c r="A28" s="23" t="s">
+        <v>541</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>512</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="23" t="s">
         <v>542</v>
       </c>
-      <c r="B28" s="24" t="s">
-        <v>513</v>
-      </c>
-      <c r="C28" s="26" t="s">
+      <c r="B29" s="24" t="s">
+        <v>571</v>
+      </c>
+      <c r="C29" s="24"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="23" t="s">
+        <v>546</v>
+      </c>
+      <c r="B30" s="24" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>543</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>574</v>
-      </c>
-      <c r="C29" s="24"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
-        <v>547</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>546</v>
-      </c>
       <c r="C30" s="24"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="33" t="s">
+        <v>556</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>555</v>
+      </c>
+      <c r="C31" s="34"/>
+    </row>
+    <row r="32" spans="1:3" ht="15">
+      <c r="A32" s="37" t="s">
         <v>557</v>
-      </c>
-      <c r="B31" s="34" t="s">
-        <v>556</v>
-      </c>
-      <c r="C31" s="34"/>
-    </row>
-    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
-        <v>560</v>
       </c>
       <c r="B32" s="38" t="s">
         <v>492</v>
       </c>
       <c r="C32" s="38" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15">
+      <c r="A33" s="37" t="s">
+        <v>558</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>522</v>
+      </c>
+      <c r="C33" s="38"/>
+    </row>
+    <row r="34" spans="1:3" ht="15">
+      <c r="A34" s="37" t="s">
+        <v>559</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>522</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15">
+      <c r="A35" s="37" t="s">
+        <v>560</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>527</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="120">
+      <c r="A36" s="37" t="s">
+        <v>561</v>
+      </c>
+      <c r="B36" s="38" t="s">
+        <v>548</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15">
+      <c r="A37" s="37" t="s">
+        <v>562</v>
+      </c>
+      <c r="B37" s="38" t="s">
+        <v>509</v>
+      </c>
+      <c r="C37" s="37" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15">
+      <c r="A38" s="37" t="s">
+        <v>568</v>
+      </c>
+      <c r="B38" s="38" t="s">
         <v>569</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
-        <v>561</v>
-      </c>
-      <c r="B33" s="38" t="s">
-        <v>523</v>
-      </c>
-      <c r="C33" s="38"/>
-    </row>
-    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="37" t="s">
-        <v>562</v>
-      </c>
-      <c r="B34" s="38" t="s">
-        <v>523</v>
-      </c>
-      <c r="C34" s="36" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="s">
-        <v>563</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>528</v>
-      </c>
-      <c r="C35" s="39" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A36" s="37" t="s">
-        <v>564</v>
-      </c>
-      <c r="B36" s="38" t="s">
-        <v>549</v>
-      </c>
-      <c r="C36" s="40" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="37" t="s">
-        <v>565</v>
-      </c>
-      <c r="B37" s="38" t="s">
-        <v>510</v>
-      </c>
-      <c r="C37" s="37" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="37" t="s">
-        <v>571</v>
-      </c>
-      <c r="B38" s="38" t="s">
-        <v>572</v>
       </c>
       <c r="C38" s="37"/>
     </row>
@@ -3218,18 +3471,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9043285-468E-4979-8BDA-14BE375A17A5}">
   <dimension ref="A1:C222"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B215" sqref="B215"/>
+    <sheetView topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="B167" sqref="B167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="173.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16.5" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3240,7 +3493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -3248,7 +3501,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -3259,7 +3512,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -3270,7 +3523,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -3281,7 +3534,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3289,7 +3542,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -3300,7 +3553,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -3311,7 +3564,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -3319,7 +3572,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -3327,7 +3580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -3338,7 +3591,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -3349,7 +3602,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -3357,7 +3610,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -3365,7 +3618,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>131</v>
       </c>
@@ -3373,7 +3626,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
@@ -3381,7 +3634,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -3389,7 +3642,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
@@ -3397,7 +3650,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
@@ -3408,7 +3661,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -3416,7 +3669,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
@@ -3427,7 +3680,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
@@ -3438,7 +3691,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -3449,7 +3702,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
@@ -3460,7 +3713,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
         <v>148</v>
       </c>
@@ -3471,7 +3724,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
         <v>47</v>
       </c>
@@ -3482,7 +3735,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
         <v>150</v>
       </c>
@@ -3493,7 +3746,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
         <v>49</v>
       </c>
@@ -3504,7 +3757,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
         <v>153</v>
       </c>
@@ -3515,7 +3768,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
         <v>155</v>
       </c>
@@ -3526,7 +3779,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
         <v>157</v>
       </c>
@@ -3537,7 +3790,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
         <v>159</v>
       </c>
@@ -3548,7 +3801,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
         <v>161</v>
       </c>
@@ -3559,7 +3812,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
         <v>163</v>
       </c>
@@ -3570,7 +3823,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
@@ -3581,7 +3834,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
         <v>165</v>
       </c>
@@ -3592,7 +3845,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
         <v>167</v>
       </c>
@@ -3603,7 +3856,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
         <v>51</v>
       </c>
@@ -3614,7 +3867,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
         <v>53</v>
       </c>
@@ -3625,7 +3878,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
         <v>55</v>
       </c>
@@ -3636,7 +3889,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
         <v>57</v>
       </c>
@@ -3647,7 +3900,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
         <v>59</v>
       </c>
@@ -3658,7 +3911,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
         <v>61</v>
       </c>
@@ -3669,7 +3922,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
         <v>172</v>
       </c>
@@ -3680,7 +3933,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
         <v>64</v>
       </c>
@@ -3691,7 +3944,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
         <v>66</v>
       </c>
@@ -3702,7 +3955,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
         <v>68</v>
       </c>
@@ -3710,7 +3963,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
         <v>97</v>
       </c>
@@ -3721,7 +3974,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
         <v>174</v>
       </c>
@@ -3732,7 +3985,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
         <v>177</v>
       </c>
@@ -3740,7 +3993,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" s="2" t="s">
         <v>179</v>
       </c>
@@ -3751,7 +4004,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
         <v>182</v>
       </c>
@@ -3762,7 +4015,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" s="2" t="s">
         <v>184</v>
       </c>
@@ -3770,7 +4023,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" s="2" t="s">
         <v>186</v>
       </c>
@@ -3781,7 +4034,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" s="2" t="s">
         <v>188</v>
       </c>
@@ -3792,7 +4045,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" s="2" t="s">
         <v>99</v>
       </c>
@@ -3803,7 +4056,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" s="2" t="s">
         <v>102</v>
       </c>
@@ -3814,7 +4067,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" s="2" t="s">
         <v>104</v>
       </c>
@@ -3825,7 +4078,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
         <v>106</v>
       </c>
@@ -3836,7 +4089,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
         <v>109</v>
       </c>
@@ -3844,7 +4097,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" s="2" t="s">
         <v>111</v>
       </c>
@@ -3852,7 +4105,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" s="2" t="s">
         <v>112</v>
       </c>
@@ -3863,7 +4116,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" s="2" t="s">
         <v>113</v>
       </c>
@@ -3874,7 +4127,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" s="2" t="s">
         <v>116</v>
       </c>
@@ -3885,7 +4138,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" s="2" t="s">
         <v>118</v>
       </c>
@@ -3896,7 +4149,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" s="2" t="s">
         <v>191</v>
       </c>
@@ -3907,7 +4160,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" s="2" t="s">
         <v>193</v>
       </c>
@@ -3918,7 +4171,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" s="2" t="s">
         <v>196</v>
       </c>
@@ -3926,7 +4179,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" s="2" t="s">
         <v>198</v>
       </c>
@@ -3937,7 +4190,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" s="2" t="s">
         <v>201</v>
       </c>
@@ -3948,7 +4201,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" s="2" t="s">
         <v>202</v>
       </c>
@@ -3959,7 +4212,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" s="2" t="s">
         <v>204</v>
       </c>
@@ -3970,7 +4223,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" s="2" t="s">
         <v>207</v>
       </c>
@@ -3981,7 +4234,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" s="2" t="s">
         <v>210</v>
       </c>
@@ -3992,7 +4245,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" s="2" t="s">
         <v>212</v>
       </c>
@@ -4003,7 +4256,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" s="2" t="s">
         <v>215</v>
       </c>
@@ -4011,7 +4264,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" s="2" t="s">
         <v>217</v>
       </c>
@@ -4022,7 +4275,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" s="2" t="s">
         <v>219</v>
       </c>
@@ -4033,7 +4286,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" s="2" t="s">
         <v>220</v>
       </c>
@@ -4044,7 +4297,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" s="2" t="s">
         <v>120</v>
       </c>
@@ -4055,7 +4308,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" s="2" t="s">
         <v>123</v>
       </c>
@@ -4063,7 +4316,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" s="2" t="s">
         <v>125</v>
       </c>
@@ -4071,7 +4324,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" s="2" t="s">
         <v>127</v>
       </c>
@@ -4079,7 +4332,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" s="2" t="s">
         <v>129</v>
       </c>
@@ -4087,7 +4340,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" s="2" t="s">
         <v>222</v>
       </c>
@@ -4098,7 +4351,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86" s="2" t="s">
         <v>225</v>
       </c>
@@ -4109,7 +4362,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" s="2" t="s">
         <v>226</v>
       </c>
@@ -4117,7 +4370,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" s="2" t="s">
         <v>228</v>
       </c>
@@ -4125,7 +4378,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" s="2" t="s">
         <v>230</v>
       </c>
@@ -4136,7 +4389,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3">
       <c r="A90" s="2" t="s">
         <v>233</v>
       </c>
@@ -4147,7 +4400,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91" s="2" t="s">
         <v>235</v>
       </c>
@@ -4155,7 +4408,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="A92" s="2" t="s">
         <v>237</v>
       </c>
@@ -4166,7 +4419,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="A93" s="2" t="s">
         <v>240</v>
       </c>
@@ -4174,7 +4427,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="A94" s="2" t="s">
         <v>242</v>
       </c>
@@ -4182,7 +4435,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="A95" s="2" t="s">
         <v>244</v>
       </c>
@@ -4193,7 +4446,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96" s="2" t="s">
         <v>247</v>
       </c>
@@ -4204,7 +4457,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3">
       <c r="A97" s="2" t="s">
         <v>248</v>
       </c>
@@ -4215,7 +4468,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3">
       <c r="A98" s="2" t="s">
         <v>251</v>
       </c>
@@ -4226,7 +4479,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3">
       <c r="A99" s="2" t="s">
         <v>252</v>
       </c>
@@ -4237,7 +4490,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3">
       <c r="A100" s="2" t="s">
         <v>255</v>
       </c>
@@ -4248,7 +4501,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3">
       <c r="A101" s="2" t="s">
         <v>256</v>
       </c>
@@ -4259,7 +4512,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3">
       <c r="A102" s="2" t="s">
         <v>258</v>
       </c>
@@ -4270,7 +4523,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3">
       <c r="A103" s="2" t="s">
         <v>261</v>
       </c>
@@ -4281,7 +4534,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3">
       <c r="A104" s="2" t="s">
         <v>262</v>
       </c>
@@ -4292,7 +4545,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3">
       <c r="A105" s="2" t="s">
         <v>264</v>
       </c>
@@ -4303,7 +4556,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3">
       <c r="A106" s="5" t="s">
         <v>265</v>
       </c>
@@ -4314,7 +4567,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3">
       <c r="A107" s="2" t="s">
         <v>267</v>
       </c>
@@ -4322,7 +4575,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="15">
       <c r="A108" s="1" t="s">
         <v>269</v>
       </c>
@@ -4333,7 +4586,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" ht="15">
       <c r="A109" s="1" t="s">
         <v>271</v>
       </c>
@@ -4344,7 +4597,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="15">
       <c r="A110" s="1" t="s">
         <v>273</v>
       </c>
@@ -4355,7 +4608,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="15">
       <c r="A111" s="1" t="s">
         <v>275</v>
       </c>
@@ -4366,7 +4619,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3">
       <c r="A112" s="1" t="s">
         <v>278</v>
       </c>
@@ -4377,7 +4630,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3">
       <c r="A113" s="2" t="s">
         <v>280</v>
       </c>
@@ -4385,7 +4638,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3">
       <c r="A114" s="2" t="s">
         <v>282</v>
       </c>
@@ -4396,7 +4649,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3">
       <c r="A115" s="2" t="s">
         <v>285</v>
       </c>
@@ -4407,7 +4660,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3">
       <c r="A116" s="2" t="s">
         <v>288</v>
       </c>
@@ -4418,7 +4671,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3">
       <c r="A117" s="2" t="s">
         <v>291</v>
       </c>
@@ -4426,7 +4679,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3">
       <c r="A118" s="2" t="s">
         <v>292</v>
       </c>
@@ -4434,7 +4687,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3">
       <c r="A119" s="2" t="s">
         <v>294</v>
       </c>
@@ -4445,7 +4698,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3">
       <c r="A120" s="2" t="s">
         <v>296</v>
       </c>
@@ -4456,7 +4709,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3">
       <c r="A121" s="2" t="s">
         <v>297</v>
       </c>
@@ -4467,7 +4720,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3">
       <c r="A122" s="2" t="s">
         <v>299</v>
       </c>
@@ -4475,7 +4728,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3">
       <c r="A123" s="2" t="s">
         <v>300</v>
       </c>
@@ -4483,7 +4736,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3">
       <c r="A124" s="2" t="s">
         <v>302</v>
       </c>
@@ -4491,7 +4744,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3">
       <c r="A125" s="2" t="s">
         <v>304</v>
       </c>
@@ -4499,7 +4752,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3">
       <c r="A126" s="2" t="s">
         <v>306</v>
       </c>
@@ -4507,7 +4760,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3">
       <c r="A127" s="1" t="s">
         <v>70</v>
       </c>
@@ -4515,7 +4768,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3">
       <c r="A128" s="1" t="s">
         <v>72</v>
       </c>
@@ -4523,7 +4776,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3">
       <c r="A129" s="1" t="s">
         <v>74</v>
       </c>
@@ -4531,7 +4784,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="15">
       <c r="A130" s="1" t="s">
         <v>76</v>
       </c>
@@ -4542,7 +4795,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="15">
       <c r="A131" s="1" t="s">
         <v>79</v>
       </c>
@@ -4553,7 +4806,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="15">
       <c r="A132" s="1" t="s">
         <v>82</v>
       </c>
@@ -4564,7 +4817,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="15">
       <c r="A133" s="1" t="s">
         <v>85</v>
       </c>
@@ -4575,7 +4828,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3">
       <c r="A134" s="6" t="s">
         <v>88</v>
       </c>
@@ -4586,7 +4839,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3">
       <c r="A135" s="1" t="s">
         <v>91</v>
       </c>
@@ -4594,7 +4847,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3">
       <c r="A136" s="2" t="s">
         <v>93</v>
       </c>
@@ -4602,7 +4855,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3">
       <c r="A137" s="2" t="s">
         <v>95</v>
       </c>
@@ -4610,7 +4863,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3">
       <c r="A138" s="2" t="s">
         <v>308</v>
       </c>
@@ -4621,7 +4874,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3">
       <c r="A139" s="2" t="s">
         <v>309</v>
       </c>
@@ -4632,7 +4885,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3">
       <c r="A140" s="2" t="s">
         <v>311</v>
       </c>
@@ -4640,7 +4893,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3">
       <c r="A141" s="6" t="s">
         <v>313</v>
       </c>
@@ -4651,7 +4904,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3">
       <c r="A142" s="6" t="s">
         <v>315</v>
       </c>
@@ -4662,7 +4915,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3">
       <c r="A143" s="6" t="s">
         <v>317</v>
       </c>
@@ -4673,7 +4926,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3">
       <c r="A144" s="2" t="s">
         <v>319</v>
       </c>
@@ -4684,7 +4937,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3">
       <c r="A145" s="2" t="s">
         <v>322</v>
       </c>
@@ -4692,7 +4945,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3">
       <c r="A146" s="2" t="s">
         <v>324</v>
       </c>
@@ -4700,7 +4953,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3">
       <c r="A147" s="2" t="s">
         <v>326</v>
       </c>
@@ -4711,7 +4964,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3">
       <c r="A148" s="2" t="s">
         <v>328</v>
       </c>
@@ -4719,7 +4972,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3">
       <c r="A149" s="2" t="s">
         <v>330</v>
       </c>
@@ -4730,7 +4983,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3">
       <c r="A150" s="2" t="s">
         <v>332</v>
       </c>
@@ -4738,7 +4991,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3">
       <c r="A151" s="2" t="s">
         <v>334</v>
       </c>
@@ -4746,7 +4999,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3">
       <c r="A152" s="2" t="s">
         <v>336</v>
       </c>
@@ -4757,7 +5010,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3">
       <c r="A153" s="2" t="s">
         <v>339</v>
       </c>
@@ -4768,7 +5021,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3">
       <c r="A154" s="2" t="s">
         <v>342</v>
       </c>
@@ -4779,7 +5032,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3">
       <c r="A155" s="2" t="s">
         <v>345</v>
       </c>
@@ -4790,7 +5043,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3">
       <c r="A156" s="2" t="s">
         <v>348</v>
       </c>
@@ -4801,7 +5054,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3">
       <c r="A157" s="2" t="s">
         <v>351</v>
       </c>
@@ -4812,7 +5065,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3">
       <c r="A158" s="2" t="s">
         <v>354</v>
       </c>
@@ -4823,7 +5076,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3">
       <c r="A159" s="2" t="s">
         <v>357</v>
       </c>
@@ -4834,7 +5087,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3">
       <c r="A160" s="2" t="s">
         <v>359</v>
       </c>
@@ -4845,7 +5098,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3">
       <c r="A161" s="2" t="s">
         <v>362</v>
       </c>
@@ -4856,7 +5109,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3">
       <c r="A162" s="2" t="s">
         <v>364</v>
       </c>
@@ -4867,7 +5120,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3">
       <c r="A163" s="2" t="s">
         <v>367</v>
       </c>
@@ -4878,7 +5131,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3">
       <c r="A164" s="2" t="s">
         <v>370</v>
       </c>
@@ -4886,7 +5139,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3">
       <c r="A165" s="2" t="s">
         <v>371</v>
       </c>
@@ -4897,7 +5150,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3">
       <c r="A166" s="2" t="s">
         <v>373</v>
       </c>
@@ -4908,7 +5161,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3">
       <c r="A167" s="2" t="s">
         <v>375</v>
       </c>
@@ -4916,7 +5169,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3">
       <c r="A168" s="2" t="s">
         <v>377</v>
       </c>
@@ -4924,7 +5177,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3">
       <c r="A169" s="2" t="s">
         <v>379</v>
       </c>
@@ -4932,7 +5185,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3">
       <c r="A170" s="2" t="s">
         <v>381</v>
       </c>
@@ -4943,7 +5196,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3">
       <c r="A171" s="2" t="s">
         <v>383</v>
       </c>
@@ -4954,7 +5207,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3">
       <c r="A172" s="2" t="s">
         <v>385</v>
       </c>
@@ -4965,7 +5218,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3">
       <c r="A173" s="2" t="s">
         <v>387</v>
       </c>
@@ -4973,7 +5226,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3">
       <c r="A174" s="2" t="s">
         <v>389</v>
       </c>
@@ -4984,7 +5237,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3">
       <c r="A175" s="2" t="s">
         <v>391</v>
       </c>
@@ -4995,7 +5248,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3">
       <c r="A176" s="2" t="s">
         <v>393</v>
       </c>
@@ -5006,7 +5259,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3">
       <c r="A177" s="2" t="s">
         <v>395</v>
       </c>
@@ -5017,7 +5270,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3">
       <c r="A178" s="2" t="s">
         <v>397</v>
       </c>
@@ -5028,7 +5281,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3">
       <c r="A179" s="2" t="s">
         <v>399</v>
       </c>
@@ -5036,7 +5289,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3">
       <c r="A180" s="2" t="s">
         <v>299</v>
       </c>
@@ -5044,7 +5297,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3">
       <c r="A181" s="2" t="s">
         <v>401</v>
       </c>
@@ -5052,7 +5305,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3">
       <c r="A182" s="2" t="s">
         <v>403</v>
       </c>
@@ -5060,7 +5313,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3">
       <c r="A183" s="2" t="s">
         <v>405</v>
       </c>
@@ -5068,7 +5321,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3">
       <c r="A184" s="2" t="s">
         <v>407</v>
       </c>
@@ -5076,7 +5329,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3">
       <c r="A185" s="2" t="s">
         <v>409</v>
       </c>
@@ -5084,7 +5337,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3">
       <c r="A186" s="2" t="s">
         <v>411</v>
       </c>
@@ -5092,7 +5345,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3">
       <c r="A187" s="2" t="s">
         <v>413</v>
       </c>
@@ -5100,7 +5353,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3">
       <c r="A188" s="2" t="s">
         <v>415</v>
       </c>
@@ -5108,7 +5361,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3">
       <c r="A189" s="2" t="s">
         <v>417</v>
       </c>
@@ -5116,7 +5369,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3">
       <c r="A190" s="2" t="s">
         <v>419</v>
       </c>
@@ -5124,7 +5377,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3">
       <c r="A191" s="2" t="s">
         <v>421</v>
       </c>
@@ -5132,7 +5385,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3">
       <c r="A192" s="2" t="s">
         <v>423</v>
       </c>
@@ -5140,7 +5393,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3">
       <c r="A193" s="2" t="s">
         <v>425</v>
       </c>
@@ -5148,7 +5401,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3">
       <c r="A194" s="2" t="s">
         <v>427</v>
       </c>
@@ -5156,7 +5409,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3">
       <c r="A195" s="2" t="s">
         <v>429</v>
       </c>
@@ -5164,7 +5417,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3">
       <c r="A196" s="2" t="s">
         <v>431</v>
       </c>
@@ -5175,7 +5428,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3">
       <c r="A197" s="2" t="s">
         <v>433</v>
       </c>
@@ -5186,7 +5439,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3">
       <c r="A198" s="2" t="s">
         <v>435</v>
       </c>
@@ -5194,7 +5447,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3">
       <c r="A199" s="2" t="s">
         <v>437</v>
       </c>
@@ -5202,7 +5455,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3">
       <c r="A200" s="2" t="s">
         <v>439</v>
       </c>
@@ -5213,7 +5466,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3">
       <c r="A201" s="2" t="s">
         <v>441</v>
       </c>
@@ -5224,7 +5477,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3">
       <c r="A202" s="2" t="s">
         <v>443</v>
       </c>
@@ -5235,7 +5488,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3">
       <c r="A203" s="2" t="s">
         <v>445</v>
       </c>
@@ -5246,7 +5499,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3">
       <c r="A204" s="2" t="s">
         <v>447</v>
       </c>
@@ -5254,7 +5507,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3">
       <c r="A205" s="2" t="s">
         <v>449</v>
       </c>
@@ -5265,7 +5518,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3">
       <c r="A206" s="2" t="s">
         <v>451</v>
       </c>
@@ -5276,7 +5529,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3">
       <c r="A207" s="2" t="s">
         <v>454</v>
       </c>
@@ -5284,7 +5537,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3">
       <c r="A208" s="2" t="s">
         <v>456</v>
       </c>
@@ -5295,7 +5548,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3">
       <c r="A209" s="2" t="s">
         <v>457</v>
       </c>
@@ -5306,7 +5559,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3">
       <c r="A210" s="2" t="s">
         <v>458</v>
       </c>
@@ -5314,7 +5567,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3">
       <c r="A211" s="2" t="s">
         <v>460</v>
       </c>
@@ -5325,7 +5578,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3">
       <c r="A212" s="2" t="s">
         <v>462</v>
       </c>
@@ -5336,7 +5589,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3">
       <c r="A213" s="2" t="s">
         <v>463</v>
       </c>
@@ -5344,7 +5597,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3">
       <c r="A214" s="2" t="s">
         <v>465</v>
       </c>
@@ -5352,7 +5605,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3">
       <c r="A215" s="2" t="s">
         <v>466</v>
       </c>
@@ -5363,7 +5616,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3">
       <c r="A216" s="2" t="s">
         <v>469</v>
       </c>
@@ -5371,7 +5624,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3">
       <c r="A217" s="1" t="s">
         <v>136</v>
       </c>
@@ -5379,7 +5632,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3">
       <c r="A218" s="1" t="s">
         <v>138</v>
       </c>
@@ -5387,7 +5640,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3">
       <c r="A219" s="1" t="s">
         <v>140</v>
       </c>
@@ -5395,7 +5648,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3">
       <c r="A220" s="2" t="s">
         <v>471</v>
       </c>
@@ -5403,7 +5656,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3">
       <c r="A221" s="2" t="s">
         <v>473</v>
       </c>
@@ -5411,7 +5664,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3">
       <c r="A222" s="2" t="s">
         <v>475</v>
       </c>
@@ -5430,4 +5683,672 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9075A9-C420-4CCD-8D59-C2DE591A132B}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="54.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="41" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
+      <c r="A2" s="42" t="s">
+        <v>484</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75">
+      <c r="A3" s="42" t="s">
+        <v>485</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="A4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>483</v>
+      </c>
+      <c r="C4" s="42"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75">
+      <c r="A5" s="10" t="s">
+        <v>578</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>577</v>
+      </c>
+      <c r="C5" s="49"/>
+    </row>
+    <row r="6" spans="1:3" ht="15.75">
+      <c r="A6" s="44" t="s">
+        <v>579</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>581</v>
+      </c>
+      <c r="C6" s="45"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
+      <c r="A7" s="44" t="s">
+        <v>580</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>582</v>
+      </c>
+      <c r="C7" s="45"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75">
+      <c r="A8" s="44" t="s">
+        <v>588</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>585</v>
+      </c>
+      <c r="C8" s="45"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75">
+      <c r="A9" s="44" t="s">
+        <v>589</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>583</v>
+      </c>
+      <c r="C9" s="45"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75">
+      <c r="A10" s="44" t="s">
+        <v>586</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>590</v>
+      </c>
+      <c r="C10" s="45"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75">
+      <c r="A11" s="44" t="s">
+        <v>587</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>584</v>
+      </c>
+      <c r="C11" s="45"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="50" t="s">
+        <v>539</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>597</v>
+      </c>
+      <c r="C12" s="51"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="52" t="s">
+        <v>533</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>532</v>
+      </c>
+      <c r="C13" s="51"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75">
+      <c r="A14" s="54" t="s">
+        <v>506</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>517</v>
+      </c>
+      <c r="C14" s="51"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75">
+      <c r="A15" s="54" t="s">
+        <v>486</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>487</v>
+      </c>
+      <c r="C15" s="54"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="31" t="s">
+        <v>520</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>531</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B11064-3E87-49B1-B841-F1DCC382A4C1}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="54.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="41" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
+      <c r="A2" s="42" t="s">
+        <v>484</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75">
+      <c r="A3" s="42" t="s">
+        <v>485</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="A4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>483</v>
+      </c>
+      <c r="C4" s="42"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75">
+      <c r="A5" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>577</v>
+      </c>
+      <c r="C5" s="43"/>
+    </row>
+    <row r="6" spans="1:3" ht="15.75">
+      <c r="A6" s="44" t="s">
+        <v>579</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>581</v>
+      </c>
+      <c r="C6" s="45"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
+      <c r="A7" s="44" t="s">
+        <v>580</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>582</v>
+      </c>
+      <c r="C7" s="45"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75">
+      <c r="A8" s="44" t="s">
+        <v>588</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>585</v>
+      </c>
+      <c r="C8" s="45"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75">
+      <c r="A9" s="44" t="s">
+        <v>589</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>583</v>
+      </c>
+      <c r="C9" s="45"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75">
+      <c r="A10" s="44" t="s">
+        <v>586</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>590</v>
+      </c>
+      <c r="C10" s="45"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75">
+      <c r="A11" s="44" t="s">
+        <v>587</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>584</v>
+      </c>
+      <c r="C11" s="45"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{EEEB8597-8F9E-427E-A065-606F94FAC02C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29F9C39-1E64-4748-B7D1-D61267A57165}">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="54.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="41" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="57" customFormat="1">
+      <c r="A2" s="16" t="s">
+        <v>484</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="57" customFormat="1">
+      <c r="A3" s="16" t="s">
+        <v>485</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="57" customFormat="1">
+      <c r="A4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>483</v>
+      </c>
+      <c r="C4" s="16"/>
+    </row>
+    <row r="5" spans="1:3" s="57" customFormat="1">
+      <c r="A5" s="58" t="s">
+        <v>486</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>487</v>
+      </c>
+      <c r="C5" s="58"/>
+    </row>
+    <row r="6" spans="1:3" s="57" customFormat="1">
+      <c r="A6" s="61" t="s">
+        <v>506</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>517</v>
+      </c>
+      <c r="C6" s="62"/>
+    </row>
+    <row r="7" spans="1:3" s="57" customFormat="1">
+      <c r="A7" s="63" t="s">
+        <v>595</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>596</v>
+      </c>
+      <c r="C7" s="62"/>
+    </row>
+    <row r="8" spans="1:3" s="57" customFormat="1">
+      <c r="A8" s="63" t="s">
+        <v>598</v>
+      </c>
+      <c r="B8" s="62" t="s">
+        <v>599</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="57" customFormat="1">
+      <c r="A9" s="61" t="s">
+        <v>520</v>
+      </c>
+      <c r="B9" s="62" t="s">
+        <v>531</v>
+      </c>
+      <c r="C9" s="62"/>
+    </row>
+    <row r="10" spans="1:3" s="57" customFormat="1">
+      <c r="A10" s="63" t="s">
+        <v>601</v>
+      </c>
+      <c r="B10" s="62" t="s">
+        <v>600</v>
+      </c>
+      <c r="C10" s="62"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75">
+      <c r="A11" s="59" t="s">
+        <v>602</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>603</v>
+      </c>
+      <c r="C11" s="64"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="59" t="s">
+        <v>604</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>599</v>
+      </c>
+      <c r="C12" s="65" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="66" t="s">
+        <v>606</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>605</v>
+      </c>
+      <c r="C13" s="66"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="69"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="71"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="69"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="71"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>611</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{95E83CE3-98F2-4D0B-9AE9-A55739CDD9C7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77054B1-93A8-4BC9-846A-A25DEE6AF6EE}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="54.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="41" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
+      <c r="A2" s="42" t="s">
+        <v>484</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75">
+      <c r="A3" s="42" t="s">
+        <v>485</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="A4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>483</v>
+      </c>
+      <c r="C4" s="42"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75">
+      <c r="A5" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="C5" s="9"/>
+    </row>
+    <row r="6" spans="1:3" ht="15.75">
+      <c r="A6" s="31" t="s">
+        <v>520</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>531</v>
+      </c>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
+      <c r="A7" s="31" t="s">
+        <v>524</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>505</v>
+      </c>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="47" t="s">
+        <v>595</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>596</v>
+      </c>
+      <c r="C8" s="48"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="61" t="s">
+        <v>506</v>
+      </c>
+      <c r="B9" s="62" t="s">
+        <v>517</v>
+      </c>
+      <c r="C9" s="62"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="61" t="s">
+        <v>520</v>
+      </c>
+      <c r="B10" s="62" t="s">
+        <v>531</v>
+      </c>
+      <c r="C10" s="62"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="63" t="s">
+        <v>601</v>
+      </c>
+      <c r="B11" s="62" t="s">
+        <v>600</v>
+      </c>
+      <c r="C11" s="62"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75">
+      <c r="A12" s="59" t="s">
+        <v>602</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>603</v>
+      </c>
+      <c r="C12" s="64"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="59" t="s">
+        <v>604</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>599</v>
+      </c>
+      <c r="C13" s="65" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="66" t="s">
+        <v>606</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>605</v>
+      </c>
+      <c r="C14" s="66"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="55" t="s">
+        <v>607</v>
+      </c>
+      <c r="B15" s="67" t="s">
+        <v>609</v>
+      </c>
+      <c r="C15" s="68" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="55" t="s">
+        <v>608</v>
+      </c>
+      <c r="B16" s="67" t="s">
+        <v>610</v>
+      </c>
+      <c r="C16" s="72" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="73" t="s">
+        <v>613</v>
+      </c>
+      <c r="B17" s="74" t="s">
+        <v>605</v>
+      </c>
+      <c r="C17" s="73"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="75" t="s">
+        <v>614</v>
+      </c>
+      <c r="B18" s="76" t="s">
+        <v>609</v>
+      </c>
+      <c r="C18" s="77" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="75" t="s">
+        <v>615</v>
+      </c>
+      <c r="B19" s="76" t="s">
+        <v>610</v>
+      </c>
+      <c r="C19" s="78" t="s">
+        <v>617</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{1C50CACA-C20A-4FD8-95B6-FD1D7EEF0097}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>